<commit_message>
Updated script to match excel doc name
</commit_message>
<xml_diff>
--- a/Credit-Metrics-Resources.xlsx
+++ b/Credit-Metrics-Resources.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bc60e2b77c84b27d/Documents/merton-model/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bc60e2b77c84b27d/Documents/Credit-Metrics-Example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="193" documentId="8_{2D1164D8-B8E8-42AD-B4D2-C3B0B4CB6E7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4FA422C8-30E2-4DC9-9FC5-4FA16DFB24F8}"/>
+  <xr:revisionPtr revIDLastSave="196" documentId="8_{2D1164D8-B8E8-42AD-B4D2-C3B0B4CB6E7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37BD8D2F-7290-4E40-BA3C-3D57F51F2264}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FA3C570F-74A3-4DDC-A218-FFFAD17FDA5C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FA3C570F-74A3-4DDC-A218-FFFAD17FDA5C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Example" sheetId="7" r:id="rId1"/>
+    <sheet name="Example.In.Excel" sheetId="7" r:id="rId1"/>
     <sheet name="Historical" sheetId="6" r:id="rId2"/>
     <sheet name="Observed.Matrix" sheetId="4" r:id="rId3"/>
     <sheet name="Fitted.Matrix" sheetId="5" r:id="rId4"/>
@@ -483,8 +483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5F5BDBB-C3C5-448F-99FE-9D33F52C3A1F}">
   <dimension ref="A2:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1470,31 +1470,31 @@
         <v>0.93162854404370421</v>
       </c>
       <c r="C42" s="2">
-        <f>IF(SUM(C31:I31) = 0, 0, IF(SUM(C31:I31) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(C31:I31))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(D31:I31))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" ref="C42:C49" si="10">IF(SUM(C31:I31) = 0, 0, IF(SUM(C31:I31) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(C31:I31))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(D31:I31))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
         <v>6.2540946364291389E-2</v>
       </c>
       <c r="D42" s="2">
-        <f>IF(SUM(D31:I31) = 0, 0, IF(SUM(D31:I31) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(D31:I31))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(E31:I31))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" ref="D42:D49" si="11">IF(SUM(D31:I31) = 0, 0, IF(SUM(D31:I31) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(D31:I31))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(E31:I31))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
         <v>4.7384536980827393E-3</v>
       </c>
       <c r="E42" s="2">
-        <f>IF(SUM(E31:I31) = 0, 0, IF(SUM(E31:I31) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(E31:I31))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(F31:I31))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" ref="E42:E49" si="12">IF(SUM(E31:I31) = 0, 0, IF(SUM(E31:I31) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(E31:I31))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(F31:I31))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
         <v>6.2669296214740177E-4</v>
       </c>
       <c r="F42" s="2">
-        <f>IF(SUM(F31:I31) = 0, 0, IF(SUM(F31:I31) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(F31:I31))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(G31:I31))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" ref="F42:F49" si="13">IF(SUM(F31:I31) = 0, 0, IF(SUM(F31:I31) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(F31:I31))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(G31:I31))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
         <v>2.9916766578312625E-4</v>
       </c>
       <c r="G42" s="2">
-        <f>IF(SUM(G31:I31) = 0, 0, IF(SUM(G31:I31) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(G31:I31))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(H31:I31))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" ref="G42:G49" si="14">IF(SUM(G31:I31) = 0, 0, IF(SUM(G31:I31) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(G31:I31))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(H31:I31))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
         <v>5.7550328357016642E-5</v>
       </c>
       <c r="H42" s="2">
-        <f>IF(SUM(H31:I31) = 0, 0, IF(SUM(H31:I31) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(H31:I31))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(I31))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" ref="H42:H49" si="15">IF(SUM(H31:I31) = 0, 0, IF(SUM(H31:I31) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(H31:I31))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(I31))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
         <v>5.6077738740482739E-5</v>
       </c>
       <c r="I42" s="2">
-        <f>IF(SUM(I31) = 0, 0, IF(SUM(I31) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(I31))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),FALSE)))</f>
+        <f t="shared" ref="I42:I49" si="16">IF(SUM(I31) = 0, 0, IF(SUM(I31) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(I31))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),FALSE)))</f>
         <v>2.1604226913396376E-4</v>
       </c>
     </row>
@@ -1503,35 +1503,35 @@
         <v>2</v>
       </c>
       <c r="B43" s="2">
-        <f>IF(SUM(B32:I32) = 0, 0, IF(SUM(B32:I32) &gt;= 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(0.99999999999999)+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(C32:I32))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE), _xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(B32:I32))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(C32:I32))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" ref="B43:B49" si="17">IF(SUM(B32:I32) = 0, 0, IF(SUM(B32:I32) &gt;= 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(0.99999999999999)+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(C32:I32))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE), _xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(B32:I32))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(C32:I32))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
         <v>9.4166706713518789E-3</v>
       </c>
       <c r="C43" s="2">
-        <f>IF(SUM(C32:I32) = 0, 0, IF(SUM(C32:I32) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(C32:I32))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(D32:I32))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="10"/>
         <v>0.92724099924494818</v>
       </c>
       <c r="D43" s="2">
-        <f>IF(SUM(D32:I32) = 0, 0, IF(SUM(D32:I32) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(D32:I32))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(E32:I32))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="11"/>
         <v>5.8071200509557816E-2</v>
       </c>
       <c r="E43" s="2">
-        <f>IF(SUM(E32:I32) = 0, 0, IF(SUM(E32:I32) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(E32:I32))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(F32:I32))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="12"/>
         <v>4.0509264367738886E-3</v>
       </c>
       <c r="F43" s="2">
-        <f>IF(SUM(F32:I32) = 0, 0, IF(SUM(F32:I32) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(F32:I32))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(G32:I32))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="13"/>
         <v>6.3182431772392574E-4</v>
       </c>
       <c r="G43" s="2">
-        <f>IF(SUM(G32:I32) = 0, 0, IF(SUM(G32:I32) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(G32:I32))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(H32:I32))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="14"/>
         <v>4.2218355365327456E-4</v>
       </c>
       <c r="H43" s="2">
-        <f>IF(SUM(H32:I32) = 0, 0, IF(SUM(H32:I32) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(H32:I32))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(I32))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="15"/>
         <v>1.1362806709749938E-4</v>
       </c>
       <c r="I43" s="2">
-        <f>IF(SUM(I32) = 0, 0, IF(SUM(I32) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(I32))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),FALSE)))</f>
+        <f t="shared" si="16"/>
         <v>2.1604226913396376E-4</v>
       </c>
     </row>
@@ -1540,35 +1540,35 @@
         <v>3</v>
       </c>
       <c r="B44" s="2">
-        <f>IF(SUM(B33:I33) = 0, 0, IF(SUM(B33:I33) &gt;= 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(0.99999999999999)+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(C33:I33))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE), _xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(B33:I33))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(C33:I33))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="17"/>
         <v>1.3996957890592965E-3</v>
       </c>
       <c r="C44" s="2">
-        <f>IF(SUM(C33:I33) = 0, 0, IF(SUM(C33:I33) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(C33:I33))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(D33:I33))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="10"/>
         <v>3.0172522547557756E-2</v>
       </c>
       <c r="D44" s="2">
-        <f>IF(SUM(D33:I33) = 0, 0, IF(SUM(D33:I33) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(D33:I33))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(E33:I33))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="11"/>
         <v>0.92328893633287934</v>
       </c>
       <c r="E44" s="2">
-        <f>IF(SUM(E33:I33) = 0, 0, IF(SUM(E33:I33) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(E33:I33))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(F33:I33))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="12"/>
         <v>3.8810342839345688E-2</v>
       </c>
       <c r="F44" s="2">
-        <f>IF(SUM(F33:I33) = 0, 0, IF(SUM(F33:I33) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(F33:I33))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(G33:I33))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="13"/>
         <v>4.1792901449902928E-3</v>
       </c>
       <c r="G44" s="2">
-        <f>IF(SUM(G33:I33) = 0, 0, IF(SUM(G33:I33) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(G33:I33))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(H33:I33))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="14"/>
         <v>1.6584812486661726E-3</v>
       </c>
       <c r="H44" s="2">
-        <f>IF(SUM(H33:I33) = 0, 0, IF(SUM(H33:I33) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(H33:I33))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(I33))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="15"/>
         <v>5.9932393555231815E-5</v>
       </c>
       <c r="I44" s="2">
-        <f>IF(SUM(I33) = 0, 0, IF(SUM(I33) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(I33))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),FALSE)))</f>
+        <f t="shared" si="16"/>
         <v>1.0512439705757926E-3</v>
       </c>
     </row>
@@ -1581,31 +1581,31 @@
         <v>2.9024691475043607E-4</v>
       </c>
       <c r="C45" s="2">
-        <f>IF(SUM(C34:I34) = 0, 0, IF(SUM(C34:I34) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(C34:I34))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(D34:I34))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="10"/>
         <v>4.1020758045884342E-3</v>
       </c>
       <c r="D45" s="2">
-        <f>IF(SUM(D34:I34) = 0, 0, IF(SUM(D34:I34) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(D34:I34))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(E34:I34))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="11"/>
         <v>7.034051922045903E-2</v>
       </c>
       <c r="E45" s="2">
-        <f>IF(SUM(E34:I34) = 0, 0, IF(SUM(E34:I34) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(E34:I34))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(F34:I34))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="12"/>
         <v>0.87995453046139183</v>
       </c>
       <c r="F45" s="2">
-        <f>IF(SUM(F34:I34) = 0, 0, IF(SUM(F34:I34) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(F34:I34))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(G34:I34))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="13"/>
         <v>3.6497780851361822E-2</v>
       </c>
       <c r="G45" s="2">
-        <f>IF(SUM(G34:I34) = 0, 0, IF(SUM(G34:I34) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(G34:I34))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(H34:I34))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="14"/>
         <v>7.2712478796691273E-3</v>
       </c>
       <c r="H45" s="2">
-        <f>IF(SUM(H34:I34) = 0, 0, IF(SUM(H34:I34) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(H34:I34))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(I34))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="15"/>
         <v>6.4225435229265835E-4</v>
       </c>
       <c r="I45" s="2">
-        <f>IF(SUM(I34) = 0, 0, IF(SUM(I34) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(I34))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),FALSE)))</f>
+        <f t="shared" si="16"/>
         <v>3.0607300734457376E-3</v>
       </c>
     </row>
@@ -1614,35 +1614,35 @@
         <v>5</v>
       </c>
       <c r="B46" s="2">
-        <f>IF(SUM(B35:I35) = 0, 0, IF(SUM(B35:I35) &gt;= 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(0.99999999999999)+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(C35:I35))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE), _xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(B35:I35))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(C35:I35))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="17"/>
         <v>-1.6303447480936484E-10</v>
       </c>
       <c r="C46" s="2">
-        <f>IF(SUM(C35:I35) = 0, 0, IF(SUM(C35:I35) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(C35:I35))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(D35:I35))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="10"/>
         <v>1.5464417908465089E-3</v>
       </c>
       <c r="D46" s="2">
-        <f>IF(SUM(D35:I35) = 0, 0, IF(SUM(D35:I35) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(D35:I35))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(E35:I35))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="11"/>
         <v>7.3463712007191262E-3</v>
       </c>
       <c r="E46" s="2">
-        <f>IF(SUM(E35:I35) = 0, 0, IF(SUM(E35:I35) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(E35:I35))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(F35:I35))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="12"/>
         <v>9.5059039940222578E-2</v>
       </c>
       <c r="F46" s="2">
-        <f>IF(SUM(F35:I35) = 0, 0, IF(SUM(F35:I35) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(F35:I35))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(G35:I35))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="13"/>
         <v>0.82003712768799097</v>
       </c>
       <c r="G46" s="2">
-        <f>IF(SUM(G35:I35) = 0, 0, IF(SUM(G35:I35) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(G35:I35))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(H35:I35))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="14"/>
         <v>6.3193573953086321E-2</v>
       </c>
       <c r="H46" s="2">
-        <f>IF(SUM(H35:I35) = 0, 0, IF(SUM(H35:I35) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(H35:I35))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(I35))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="15"/>
         <v>6.1419599967489497E-3</v>
       </c>
       <c r="I46" s="2">
-        <f>IF(SUM(I35) = 0, 0, IF(SUM(I35) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(I35))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),FALSE)))</f>
+        <f t="shared" si="16"/>
         <v>1.8686793056053738E-2</v>
       </c>
     </row>
@@ -1651,35 +1651,35 @@
         <v>6</v>
       </c>
       <c r="B47" s="2">
-        <f>IF(SUM(B36:I36) = 0, 0, IF(SUM(B36:I36) &gt;= 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(0.99999999999999)+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(C36:I36))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE), _xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(B36:I36))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(C36:I36))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="17"/>
         <v>-1.6303447480936484E-10</v>
       </c>
       <c r="C47" s="2">
-        <f>IF(SUM(C36:I36) = 0, 0, IF(SUM(C36:I36) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(C36:I36))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(D36:I36))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="10"/>
         <v>7.139477173988551E-4</v>
       </c>
       <c r="D47" s="2">
-        <f>IF(SUM(D36:I36) = 0, 0, IF(SUM(D36:I36) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(D36:I36))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(E36:I36))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="11"/>
         <v>3.4102597459108042E-3</v>
       </c>
       <c r="E47" s="2">
-        <f>IF(SUM(E36:I36) = 0, 0, IF(SUM(E36:I36) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(E36:I36))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(F36:I36))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="12"/>
         <v>5.9459443767070352E-3</v>
       </c>
       <c r="F47" s="2">
-        <f>IF(SUM(F36:I36) = 0, 0, IF(SUM(F36:I36) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(F36:I36))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(G36:I36))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="13"/>
         <v>8.585937702673796E-2</v>
       </c>
       <c r="G47" s="2">
-        <f>IF(SUM(G36:I36) = 0, 0, IF(SUM(G36:I36) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(G36:I36))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(H36:I36))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="14"/>
         <v>0.83677328770934145</v>
       </c>
       <c r="H47" s="2">
-        <f>IF(SUM(H36:I36) = 0, 0, IF(SUM(H36:I36) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(H36:I36))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(I36))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="15"/>
         <v>3.0340575116948564E-2</v>
       </c>
       <c r="I47" s="2">
-        <f>IF(SUM(I36) = 0, 0, IF(SUM(I36) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(I36))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),FALSE)))</f>
+        <f t="shared" si="16"/>
         <v>8.0790859421504782E-2</v>
       </c>
     </row>
@@ -1688,35 +1688,35 @@
         <v>7</v>
       </c>
       <c r="B48" s="2">
-        <f>IF(SUM(B37:I37) = 0, 0, IF(SUM(B37:I37) &gt;= 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(0.99999999999999)+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(C37:I37))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE), _xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(B37:I37))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(C37:I37))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="17"/>
         <v>-1.6303447480936484E-10</v>
       </c>
       <c r="C48" s="2">
-        <f>IF(SUM(C37:I37) = 0, 0, IF(SUM(C37:I37) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(C37:I37))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(D37:I37))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="10"/>
         <v>1.467460017871014E-4</v>
       </c>
       <c r="D48" s="2">
-        <f>IF(SUM(D37:I37) = 0, 0, IF(SUM(D37:I37) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(D37:I37))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(E37:I37))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="11"/>
         <v>1.3996957890591855E-3</v>
       </c>
       <c r="E48" s="2">
-        <f>IF(SUM(E37:I37) = 0, 0, IF(SUM(E37:I37) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(E37:I37))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(F37:I37))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="12"/>
         <v>4.046934386489287E-3</v>
       </c>
       <c r="F48" s="2">
-        <f>IF(SUM(F37:I37) = 0, 0, IF(SUM(F37:I37) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(F37:I37))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(G37:I37))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="13"/>
         <v>3.2971595260099296E-2</v>
       </c>
       <c r="G48" s="2">
-        <f>IF(SUM(G37:I37) = 0, 0, IF(SUM(G37:I37) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(G37:I37))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(H37:I37))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="14"/>
         <v>0.14120026370810868</v>
       </c>
       <c r="H48" s="2">
-        <f>IF(SUM(H37:I37) = 0, 0, IF(SUM(H37:I37) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(H37:I37))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(I37))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="15"/>
         <v>0.65602204451956436</v>
       </c>
       <c r="I48" s="2">
-        <f>IF(SUM(I37) = 0, 0, IF(SUM(I37) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(I37))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),FALSE)))</f>
+        <f t="shared" si="16"/>
         <v>0.24746485051173994</v>
       </c>
     </row>
@@ -1725,35 +1725,35 @@
         <v>8</v>
       </c>
       <c r="B49" s="2">
-        <f>IF(SUM(B38:I38) = 0, 0, IF(SUM(B38:I38) &gt;= 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(0.99999999999999)+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(C38:I38))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE), _xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(B38:I38))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(C38:I38))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="17"/>
         <v>-1.6188650420190243E-10</v>
       </c>
       <c r="C49" s="2">
-        <f>IF(SUM(C38:I38) = 0, 0, IF(SUM(C38:I38) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(C38:I38))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(D38:I38))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="10"/>
         <v>-1.6199663832594524E-10</v>
       </c>
       <c r="D49" s="2">
-        <f>IF(SUM(D38:I38) = 0, 0, IF(SUM(D38:I38) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(D38:I38))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(E38:I38))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="11"/>
         <v>-1.6212298170614758E-10</v>
       </c>
       <c r="E49" s="2">
-        <f>IF(SUM(E38:I38) = 0, 0, IF(SUM(E38:I38) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(E38:I38))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(F38:I38))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="12"/>
         <v>-1.6227152954684243E-10</v>
       </c>
       <c r="F49" s="2">
-        <f>IF(SUM(F38:I38) = 0, 0, IF(SUM(F38:I38) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(F38:I38))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(G38:I38))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="13"/>
         <v>-1.6245338407827603E-10</v>
       </c>
       <c r="G49" s="2">
-        <f>IF(SUM(G38:I38) = 0, 0, IF(SUM(G38:I38) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(G38:I38))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(H38:I38))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="14"/>
         <v>-1.6268941749331134E-10</v>
       </c>
       <c r="H49" s="2">
-        <f>IF(SUM(H38:I38) = 0, 0, IF(SUM(H38:I38) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(H38:I38))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)-_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(I38))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),TRUE)))</f>
+        <f t="shared" si="15"/>
         <v>-1.6303447480936484E-10</v>
       </c>
       <c r="I49" s="2">
-        <f>IF(SUM(I38) = 0, 0, IF(SUM(I38) = 1, 1,_xlfn.NORM.S.DIST((_xlfn.NORM.S.INV(SUM(I38))+SQRT($H$2)*-$D$2)/SQRT(1-$H$2),FALSE)))</f>
+        <f t="shared" si="16"/>
         <v>1.0544975499729198E-9</v>
       </c>
     </row>
@@ -2595,7 +2595,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="A1:I9"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>